<commit_message>
Added 222 North Lasalle
</commit_message>
<xml_diff>
--- a/data/160 and 333.xlsx
+++ b/data/160 and 333.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{77D0D91E-1EB6-4B0F-A708-1FD88462194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75DE234A-29BE-4FD4-8A14-6069F71F0669}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{77D0D91E-1EB6-4B0F-A708-1FD88462194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB699F7A-A6DC-4404-9B06-B8F73C1A9CD8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
   </bookViews>
   <sheets>
     <sheet name="160 Spear " sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="77">
   <si>
     <t>Building Level Interventions</t>
   </si>
@@ -289,6 +289,30 @@
   </si>
   <si>
     <t xml:space="preserve"> Capex </t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>160 Spear</t>
+  </si>
+  <si>
+    <t>Heating &amp; Cooling &amp; Base</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>Heating &amp; Cooling</t>
+  </si>
+  <si>
+    <t>Test Name</t>
   </si>
 </sst>
 </file>
@@ -594,7 +618,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -669,6 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -830,14 +855,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -875,7 +896,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -981,7 +1002,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1123,7 +1144,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1131,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF149E70-DC8C-4A8D-84BB-B0051DA57024}">
-  <dimension ref="A2:N45"/>
+  <dimension ref="A2:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1818,7 @@
       <c r="M32" s="22"/>
       <c r="N32" s="23"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1812,7 +1833,7 @@
       <c r="M33" s="12"/>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1827,7 +1848,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1842,7 +1863,7 @@
       <c r="M35" s="12"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1857,7 +1878,7 @@
       <c r="M36" s="12"/>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1872,7 +1893,7 @@
       <c r="M37" s="12"/>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1887,7 +1908,7 @@
       <c r="M38" s="12"/>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1902,7 +1923,7 @@
       <c r="M39" s="12"/>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
         <v>20</v>
@@ -1919,7 +1940,7 @@
       <c r="M40" s="12"/>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
         <v>20</v>
@@ -1938,7 +1959,7 @@
       <c r="M41" s="12"/>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -1953,10 +1974,456 @@
       <c r="M42" s="12"/>
       <c r="N42" s="16"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="36">
+        <v>45390</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="126" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="18">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48">
+        <v>35000</v>
+      </c>
+      <c r="H48" t="s">
+        <v>65</v>
+      </c>
+      <c r="I48">
+        <v>0.04</v>
+      </c>
+      <c r="J48">
+        <v>0.04</v>
+      </c>
+      <c r="K48" t="s">
+        <v>66</v>
+      </c>
+      <c r="M48" s="19"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="23"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="18">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49">
+        <v>120000</v>
+      </c>
+      <c r="H49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49">
+        <v>0.01</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49" t="s">
+        <v>66</v>
+      </c>
+      <c r="M49" s="19"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="23"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="18">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>650000</v>
+      </c>
+      <c r="H50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50">
+        <v>0.1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50" t="s">
+        <v>66</v>
+      </c>
+      <c r="M50" s="19"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="23"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="18">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51">
+        <v>85000</v>
+      </c>
+      <c r="H51" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51">
+        <v>0.5</v>
+      </c>
+      <c r="J51">
+        <v>-0.5</v>
+      </c>
+      <c r="K51" t="s">
+        <v>66</v>
+      </c>
+      <c r="M51" s="19"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="23"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="18">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52">
+        <v>1000000</v>
+      </c>
+      <c r="H52" t="s">
+        <v>65</v>
+      </c>
+      <c r="I52">
+        <v>0.02</v>
+      </c>
+      <c r="J52">
+        <v>0.02</v>
+      </c>
+      <c r="K52" t="s">
+        <v>66</v>
+      </c>
+      <c r="M52" s="19"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="23"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="18">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53">
+        <v>10000000</v>
+      </c>
+      <c r="H53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I53">
+        <v>0.05</v>
+      </c>
+      <c r="J53">
+        <v>0.05</v>
+      </c>
+      <c r="K53" t="s">
+        <v>66</v>
+      </c>
+      <c r="M53" s="19"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="23"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="18">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54">
+        <v>2750000</v>
+      </c>
+      <c r="H54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>-1</v>
+      </c>
+      <c r="K54" t="s">
+        <v>66</v>
+      </c>
+      <c r="M54" s="19"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="23"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="18">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55">
+        <v>1500000</v>
+      </c>
+      <c r="H55" t="s">
+        <v>68</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>-1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>66</v>
+      </c>
+      <c r="M55" s="19"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="23"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="18">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56">
+        <v>230000</v>
+      </c>
+      <c r="H56" t="s">
+        <v>68</v>
+      </c>
+      <c r="I56">
+        <v>0.02</v>
+      </c>
+      <c r="J56">
+        <v>0.02</v>
+      </c>
+      <c r="K56" t="s">
+        <v>66</v>
+      </c>
+      <c r="M56" s="19"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="23"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="18">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>1000000</v>
+      </c>
+      <c r="H57" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>-1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>66</v>
+      </c>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1967,7 +2434,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M18:M42" xr:uid="{25478E18-0184-44CC-B842-F228497F826A}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F42 D18:D43" xr:uid="{19480D23-33C3-4743-91EA-3363E4F8A8EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F42 D18:D43 O48:O57 B48:B57" xr:uid="{19480D23-33C3-4743-91EA-3363E4F8A8EB}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1981,7 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963D9F0D-2B14-4150-932F-0DCDDE43FCB8}">
   <dimension ref="A2:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>